<commit_message>
Added books with ISBN ID, removed images
</commit_message>
<xml_diff>
--- a/Book_Database.xlsx
+++ b/Book_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saswata\Documents\Github_Repos\biblioteca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B372B91E-3D9C-44DA-8DCF-62D0EC759EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE81B12-54A7-47D3-A415-CECF47600D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Book Name</t>
   </si>
@@ -49,65 +49,56 @@
     <t>Back Cover</t>
   </si>
   <si>
-    <t>Sapiens</t>
-  </si>
-  <si>
-    <t>The Alchemist</t>
-  </si>
-  <si>
-    <t>Sapiens: A Brief History of Humankind</t>
-  </si>
-  <si>
-    <t>O Alquimista</t>
-  </si>
-  <si>
-    <t>Yuval Noah Harari</t>
-  </si>
-  <si>
-    <t>Paulo Coelho</t>
-  </si>
-  <si>
-    <t>Penguin Random House</t>
-  </si>
-  <si>
-    <t>HarperOne</t>
-  </si>
-  <si>
     <t>Non-Fiction</t>
   </si>
   <si>
-    <t>Fiction</t>
-  </si>
-  <si>
     <t>History</t>
   </si>
   <si>
-    <t>Philosophical Novel</t>
-  </si>
-  <si>
     <t>Paperback</t>
   </si>
   <si>
-    <t>Insert Image</t>
-  </si>
-  <si>
-    <t>sapiens_front.jpg</t>
-  </si>
-  <si>
-    <t>sapiens_back.jpg</t>
-  </si>
-  <si>
     <t>Book Name (Original Language)</t>
   </si>
   <si>
     <t>ISBN</t>
+  </si>
+  <si>
+    <t>978-93-5520-982-5</t>
+  </si>
+  <si>
+    <t>Bollywood, Box Office and Beyond</t>
+  </si>
+  <si>
+    <t>Box Office and Beyond</t>
+  </si>
+  <si>
+    <t>Lata Jha</t>
+  </si>
+  <si>
+    <t>Rupa</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Games People Play</t>
+  </si>
+  <si>
+    <t>Eric Berne</t>
+  </si>
+  <si>
+    <t>978-0-241-25747-0</t>
+  </si>
+  <si>
+    <t>Penguin Life</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,12 +107,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,15 +161,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -476,123 +481,118 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3">
         <v>499</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="4">
+        <v>199</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3">
-        <v>350</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="I3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Language field to database and Streamlit UI
</commit_message>
<xml_diff>
--- a/Book_Database.xlsx
+++ b/Book_Database.xlsx
@@ -1,116 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saswata\Documents\Github_Repos\biblioteca\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E959E6C2-2129-4934-8EA8-28B0958C1BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t>Book Name</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Publisher</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Fiction / Non-Fiction</t>
-  </si>
-  <si>
-    <t>Genre</t>
-  </si>
-  <si>
-    <t>Format</t>
-  </si>
-  <si>
-    <t>Non-Fiction</t>
-  </si>
-  <si>
-    <t>History</t>
-  </si>
-  <si>
-    <t>Paperback</t>
-  </si>
-  <si>
-    <t>Bollywood, Box Office and Beyond</t>
-  </si>
-  <si>
-    <t>Lata Jha</t>
-  </si>
-  <si>
-    <t>Rupa</t>
-  </si>
-  <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>Games People Play</t>
-  </si>
-  <si>
-    <t>Eric Berne</t>
-  </si>
-  <si>
-    <t>Penguin Life</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ISBN</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -143,41 +73,94 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -467,103 +450,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:H3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col width="32.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="26.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="22.42578125" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="18.85546875" bestFit="1" customWidth="1" min="6" max="7"/>
+    <col width="16.5703125" bestFit="1" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Book Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ISBN</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Publisher</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Fiction / Non-Fiction</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Genre</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Format</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Language</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5">
+    <row r="2" ht="65.25" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Games People Play</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Eric Berne</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="n">
         <v>9780241257470</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Penguin Life</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>499</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>9</v>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Non-Fiction</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>History</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="6">
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Bollywood, Box Office and Beyond</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Lata Jha</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="n">
         <v>9789355209825</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Rupa</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
         <v>199</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>9</v>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>Non-Fiction</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Amar Dekha Poka-Makor</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Gopal Chandra Bhattacharya</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>9788129507969</v>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Dey's Publishing</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>Non-Fiction</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>Animal Kingdom</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>Hard-Cover</t>
+        </is>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C4" display="https://isbnsearch.org/isbn/9788129507969" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>